<commit_message>
lots of stuff added
</commit_message>
<xml_diff>
--- a/L82V_muts_activity.xlsx
+++ b/L82V_muts_activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlho/Documents/Shakh Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24CAC4D-D89C-014C-9E74-CC000ABAD244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CD6819-C49B-8A4D-BC47-45CFAA8C974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1060" windowWidth="28260" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,19 +203,7 @@
     <t>L168G T2</t>
   </si>
   <si>
-    <t>112/168G T1</t>
-  </si>
-  <si>
     <t>delayed</t>
-  </si>
-  <si>
-    <t>112/168G T2</t>
-  </si>
-  <si>
-    <t>117/164G T1</t>
-  </si>
-  <si>
-    <t>117/164G T2</t>
   </si>
   <si>
     <t>D118N T1</t>
@@ -228,6 +216,18 @@
   </si>
   <si>
     <t>L82V T2</t>
+  </si>
+  <si>
+    <t>112-168G T1</t>
+  </si>
+  <si>
+    <t>112-168G T2</t>
+  </si>
+  <si>
+    <t>117-164G T1</t>
+  </si>
+  <si>
+    <t>117-164G T2</t>
   </si>
 </sst>
 </file>
@@ -42154,8 +42154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R431"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42246,35 +42246,35 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>-SLOPE(B2:B8,$J$2:$J$8)</f>
+        <f t="shared" ref="K2:R2" si="0">-SLOPE(B2:B8,$J$2:$J$8)</f>
         <v>4.2857142857142892E-2</v>
       </c>
       <c r="L2">
-        <f>-SLOPE(C2:C8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.2999999999999884E-2</v>
       </c>
       <c r="M2">
-        <f>-SLOPE(D2:D8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.5999999999999741E-2</v>
       </c>
       <c r="N2">
-        <f>-SLOPE(E2:E8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.7285714285714311E-2</v>
       </c>
       <c r="O2">
-        <f>-SLOPE(F2:F8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.3857142857142877E-2</v>
       </c>
       <c r="P2">
-        <f>-SLOPE(G2:G8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>2.7000000000000021E-2</v>
       </c>
       <c r="Q2">
-        <f>-SLOPE(H2:H8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.0428571428571451E-2</v>
       </c>
       <c r="R2">
-        <f>-SLOPE(I2:I8,$J$2:$J$8)</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000023E-2</v>
       </c>
     </row>
@@ -42307,7 +42307,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:J26" si="0">HOUR(A3)*60+MINUTE(A3)+SECOND(A3)/60</f>
+        <f t="shared" ref="J3:J26" si="1">HOUR(A3)*60+MINUTE(A3)+SECOND(A3)/60</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="K3">
@@ -42372,7 +42372,7 @@
         <v>0.7</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -42405,7 +42405,7 @@
         <v>0.69799999999999995</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
@@ -42438,7 +42438,7 @@
         <v>0.69599999999999995</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -42471,7 +42471,7 @@
         <v>0.69299999999999995</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -42504,7 +42504,7 @@
         <v>0.69199999999999995</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -42537,7 +42537,7 @@
         <v>0.68899999999999995</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -42570,7 +42570,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -42603,7 +42603,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
     </row>
@@ -42636,7 +42636,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -42669,7 +42669,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
     </row>
@@ -42702,7 +42702,7 @@
         <v>0.68100000000000005</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -42735,7 +42735,7 @@
         <v>0.68</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0833333333333333</v>
       </c>
     </row>
@@ -42768,7 +42768,7 @@
         <v>0.67800000000000005</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
     </row>
@@ -42801,7 +42801,7 @@
         <v>0.67700000000000005</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -42834,7 +42834,7 @@
         <v>0.67600000000000005</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -42867,7 +42867,7 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4166666666666667</v>
       </c>
     </row>
@@ -42900,7 +42900,7 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -42933,7 +42933,7 @@
         <v>0.67400000000000004</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5833333333333335</v>
       </c>
     </row>
@@ -42966,7 +42966,7 @@
         <v>0.67300000000000004</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666665</v>
       </c>
     </row>
@@ -42999,7 +42999,7 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -43032,7 +43032,7 @@
         <v>0.67</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
     </row>
@@ -43065,7 +43065,7 @@
         <v>0.66900000000000004</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9166666666666665</v>
       </c>
     </row>
@@ -43098,7 +43098,7 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -43192,27 +43192,27 @@
         <v>4.2857142857142892E-2</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29" si="1">-SLOPE(D29:D35,$J$2:$J$8)</f>
+        <f t="shared" ref="M29" si="2">-SLOPE(D29:D35,$J$2:$J$8)</f>
         <v>5.1428571428571469E-2</v>
       </c>
       <c r="N29">
-        <f t="shared" ref="N29" si="2">-SLOPE(E29:E35,$J$2:$J$8)</f>
+        <f t="shared" ref="N29" si="3">-SLOPE(E29:E35,$J$2:$J$8)</f>
         <v>4.1142857142857175E-2</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29" si="3">-SLOPE(F29:F35,$J$2:$J$8)</f>
+        <f t="shared" ref="O29" si="4">-SLOPE(F29:F35,$J$2:$J$8)</f>
         <v>3.6857142857142887E-2</v>
       </c>
       <c r="P29">
-        <f t="shared" ref="P29" si="4">-SLOPE(G29:G35,$J$2:$J$8)</f>
+        <f t="shared" ref="P29" si="5">-SLOPE(G29:G35,$J$2:$J$8)</f>
         <v>3.985714285714289E-2</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q29" si="5">-SLOPE(H29:H35,$J$2:$J$8)</f>
+        <f t="shared" ref="Q29" si="6">-SLOPE(H29:H35,$J$2:$J$8)</f>
         <v>3.6000000000000025E-2</v>
       </c>
       <c r="R29">
-        <f t="shared" ref="R29" si="6">-SLOPE(I29:I35,$J$2:$J$8)</f>
+        <f t="shared" ref="R29" si="7">-SLOPE(I29:I35,$J$2:$J$8)</f>
         <v>3.6000000000000032E-2</v>
       </c>
     </row>
@@ -44002,27 +44002,27 @@
         <v>4.4571428571428609E-2</v>
       </c>
       <c r="M56">
-        <f t="shared" ref="M56" si="7">-SLOPE(D56:D62,$J$2:$J$8)</f>
+        <f t="shared" ref="M56" si="8">-SLOPE(D56:D62,$J$2:$J$8)</f>
         <v>2.1857142857142874E-2</v>
       </c>
       <c r="N56">
-        <f t="shared" ref="N56" si="8">-SLOPE(E56:E62,$J$2:$J$8)</f>
+        <f t="shared" ref="N56" si="9">-SLOPE(E56:E62,$J$2:$J$8)</f>
         <v>1.6714285714285727E-2</v>
       </c>
       <c r="O56">
-        <f t="shared" ref="O56" si="9">-SLOPE(F56:F62,$J$2:$J$8)</f>
+        <f t="shared" ref="O56" si="10">-SLOPE(F56:F62,$J$2:$J$8)</f>
         <v>4.4571428571428609E-2</v>
       </c>
       <c r="P56">
-        <f t="shared" ref="P56" si="10">-SLOPE(G56:G62,$J$2:$J$8)</f>
+        <f t="shared" ref="P56" si="11">-SLOPE(G56:G62,$J$2:$J$8)</f>
         <v>4.0714285714285738E-2</v>
       </c>
       <c r="Q56">
-        <f t="shared" ref="Q56" si="11">-SLOPE(H56:H62,$J$2:$J$8)</f>
+        <f t="shared" ref="Q56" si="12">-SLOPE(H56:H62,$J$2:$J$8)</f>
         <v>4.8857142857142891E-2</v>
       </c>
       <c r="R56">
-        <f t="shared" ref="R56" si="12">-SLOPE(I56:I62,$J$2:$J$8)</f>
+        <f t="shared" ref="R56" si="13">-SLOPE(I56:I62,$J$2:$J$8)</f>
         <v>4.6714285714285757E-2</v>
       </c>
     </row>
@@ -44812,27 +44812,27 @@
         <v>3.4285714285714308E-2</v>
       </c>
       <c r="M83">
-        <f t="shared" ref="M83" si="13">-SLOPE(D83:D89,$J$2:$J$8)</f>
+        <f t="shared" ref="M83" si="14">-SLOPE(D83:D89,$J$2:$J$8)</f>
         <v>2.8285714285714306E-2</v>
       </c>
       <c r="N83">
-        <f t="shared" ref="N83" si="14">-SLOPE(E83:E89,$J$2:$J$8)</f>
+        <f t="shared" ref="N83" si="15">-SLOPE(E83:E89,$J$2:$J$8)</f>
         <v>3.1714285714285743E-2</v>
       </c>
       <c r="O83">
-        <f t="shared" ref="O83" si="15">-SLOPE(F83:F89,$J$2:$J$8)</f>
+        <f t="shared" ref="O83" si="16">-SLOPE(F83:F89,$J$2:$J$8)</f>
         <v>3.3000000000000022E-2</v>
       </c>
       <c r="P83">
-        <f t="shared" ref="P83" si="16">-SLOPE(G83:G89,$J$2:$J$8)</f>
+        <f t="shared" ref="P83" si="17">-SLOPE(G83:G89,$J$2:$J$8)</f>
         <v>4.0714285714285744E-2</v>
       </c>
       <c r="Q83">
-        <f t="shared" ref="Q83" si="17">-SLOPE(H83:H89,$J$2:$J$8)</f>
+        <f t="shared" ref="Q83" si="18">-SLOPE(H83:H89,$J$2:$J$8)</f>
         <v>3.1714285714285743E-2</v>
       </c>
       <c r="R83">
-        <f t="shared" ref="R83" si="18">-SLOPE(I83:I89,$J$2:$J$8)</f>
+        <f t="shared" ref="R83" si="19">-SLOPE(I83:I89,$J$2:$J$8)</f>
         <v>1.9714285714285729E-2</v>
       </c>
     </row>
@@ -45622,27 +45622,27 @@
         <v>3.2142857142857167E-2</v>
       </c>
       <c r="M110">
-        <f t="shared" ref="M110" si="19">-SLOPE(D110:D116,$J$2:$J$8)</f>
+        <f t="shared" ref="M110" si="20">-SLOPE(D110:D116,$J$2:$J$8)</f>
         <v>9.4714285714285792E-2</v>
       </c>
       <c r="N110">
-        <f t="shared" ref="N110" si="20">-SLOPE(E110:E116,$J$2:$J$8)</f>
+        <f t="shared" ref="N110" si="21">-SLOPE(E110:E116,$J$2:$J$8)</f>
         <v>4.0714285714285744E-2</v>
       </c>
       <c r="O110">
-        <f t="shared" ref="O110" si="21">-SLOPE(F110:F116,$J$2:$J$8)</f>
+        <f t="shared" ref="O110" si="22">-SLOPE(F110:F116,$J$2:$J$8)</f>
         <v>3.0428571428571454E-2</v>
       </c>
       <c r="P110">
-        <f t="shared" ref="P110" si="22">-SLOPE(G110:G116,$J$2:$J$8)</f>
+        <f t="shared" ref="P110" si="23">-SLOPE(G110:G116,$J$2:$J$8)</f>
         <v>3.1714285714285737E-2</v>
       </c>
       <c r="Q110">
-        <f t="shared" ref="Q110" si="23">-SLOPE(H110:H116,$J$2:$J$8)</f>
+        <f t="shared" ref="Q110" si="24">-SLOPE(H110:H116,$J$2:$J$8)</f>
         <v>3.2571428571428598E-2</v>
       </c>
       <c r="R110">
-        <f t="shared" ref="R110" si="24">-SLOPE(I110:I116,$J$2:$J$8)</f>
+        <f t="shared" ref="R110" si="25">-SLOPE(I110:I116,$J$2:$J$8)</f>
         <v>3.0428571428571454E-2</v>
       </c>
     </row>
@@ -46432,27 +46432,27 @@
         <v>2.4857142857142876E-2</v>
       </c>
       <c r="M137">
-        <f t="shared" ref="M137" si="25">-SLOPE(D137:D143,$J$2:$J$8)</f>
+        <f t="shared" ref="M137" si="26">-SLOPE(D137:D143,$J$2:$J$8)</f>
         <v>2.9571428571428592E-2</v>
       </c>
       <c r="N137">
-        <f t="shared" ref="N137" si="26">-SLOPE(E137:E143,$J$2:$J$8)</f>
+        <f t="shared" ref="N137" si="27">-SLOPE(E137:E143,$J$2:$J$8)</f>
         <v>1.8857142857142871E-2</v>
       </c>
       <c r="O137">
-        <f t="shared" ref="O137" si="27">-SLOPE(F137:F143,$J$2:$J$8)</f>
+        <f t="shared" ref="O137" si="28">-SLOPE(F137:F143,$J$2:$J$8)</f>
         <v>2.4857142857142876E-2</v>
       </c>
       <c r="P137">
-        <f t="shared" ref="P137" si="28">-SLOPE(G137:G143,$J$2:$J$8)</f>
+        <f t="shared" ref="P137" si="29">-SLOPE(G137:G143,$J$2:$J$8)</f>
         <v>2.5285714285714307E-2</v>
       </c>
       <c r="Q137">
-        <f t="shared" ref="Q137" si="29">-SLOPE(H137:H143,$J$2:$J$8)</f>
+        <f t="shared" ref="Q137" si="30">-SLOPE(H137:H143,$J$2:$J$8)</f>
         <v>1.9285714285714298E-2</v>
       </c>
       <c r="R137">
-        <f t="shared" ref="R137" si="30">-SLOPE(I137:I143,$J$2:$J$8)</f>
+        <f t="shared" ref="R137" si="31">-SLOPE(I137:I143,$J$2:$J$8)</f>
         <v>3.0000000000000023E-2</v>
       </c>
     </row>
@@ -47242,27 +47242,27 @@
         <v>2.7857142857142875E-2</v>
       </c>
       <c r="M164">
-        <f t="shared" ref="M164" si="31">-SLOPE(D164:D170,$J$2:$J$8)</f>
+        <f t="shared" ref="M164" si="32">-SLOPE(D164:D170,$J$2:$J$8)</f>
         <v>2.7000000000000021E-2</v>
       </c>
       <c r="N164">
-        <f t="shared" ref="N164" si="32">-SLOPE(E164:E170,$J$2:$J$8)</f>
+        <f t="shared" ref="N164" si="33">-SLOPE(E164:E170,$J$2:$J$8)</f>
         <v>1.7142857142857153E-3</v>
       </c>
       <c r="O164">
-        <f t="shared" ref="O164" si="33">-SLOPE(F164:F170,$J$2:$J$8)</f>
+        <f t="shared" ref="O164" si="34">-SLOPE(F164:F170,$J$2:$J$8)</f>
         <v>2.9571428571428592E-2</v>
       </c>
       <c r="P164">
-        <f t="shared" ref="P164" si="34">-SLOPE(G164:G170,$J$2:$J$8)</f>
+        <f t="shared" ref="P164" si="35">-SLOPE(G164:G170,$J$2:$J$8)</f>
         <v>2.8285714285714306E-2</v>
       </c>
       <c r="Q164">
-        <f t="shared" ref="Q164" si="35">-SLOPE(H164:H170,$J$2:$J$8)</f>
+        <f t="shared" ref="Q164" si="36">-SLOPE(H164:H170,$J$2:$J$8)</f>
         <v>2.1857142857142731E-2</v>
       </c>
       <c r="R164">
-        <f t="shared" ref="R164" si="36">-SLOPE(I164:I170,$J$2:$J$8)</f>
+        <f t="shared" ref="R164" si="37">-SLOPE(I164:I170,$J$2:$J$8)</f>
         <v>1.7571428571428346E-2</v>
       </c>
     </row>
@@ -48052,27 +48052,27 @@
         <v>1.8857142857142871E-2</v>
       </c>
       <c r="M191">
-        <f t="shared" ref="M191" si="37">-SLOPE(D191:D197,$J$2:$J$8)</f>
+        <f t="shared" ref="M191" si="38">-SLOPE(D191:D197,$J$2:$J$8)</f>
         <v>3.685714285714288E-2</v>
       </c>
       <c r="N191">
-        <f t="shared" ref="N191" si="38">-SLOPE(E191:E197,$J$2:$J$8)</f>
+        <f t="shared" ref="N191" si="39">-SLOPE(E191:E197,$J$2:$J$8)</f>
         <v>3.4285714285714308E-2</v>
       </c>
       <c r="O191">
-        <f t="shared" ref="O191" si="39">-SLOPE(F191:F197,$J$2:$J$8)</f>
+        <f t="shared" ref="O191" si="40">-SLOPE(F191:F197,$J$2:$J$8)</f>
         <v>3.1285714285714313E-2</v>
       </c>
       <c r="P191">
-        <f t="shared" ref="P191" si="40">-SLOPE(G191:G197,$J$2:$J$8)</f>
+        <f t="shared" ref="P191" si="41">-SLOPE(G191:G197,$J$2:$J$8)</f>
         <v>2.5714285714285735E-2</v>
       </c>
       <c r="Q191">
-        <f t="shared" ref="Q191" si="41">-SLOPE(H191:H197,$J$2:$J$8)</f>
+        <f t="shared" ref="Q191" si="42">-SLOPE(H191:H197,$J$2:$J$8)</f>
         <v>3.985714285714289E-2</v>
       </c>
       <c r="R191">
-        <f t="shared" ref="R191" si="42">-SLOPE(I191:I197,$J$2:$J$8)</f>
+        <f t="shared" ref="R191" si="43">-SLOPE(I191:I197,$J$2:$J$8)</f>
         <v>3.7285714285714311E-2</v>
       </c>
     </row>
@@ -48774,7 +48774,7 @@
     </row>
     <row r="217" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>18</v>
@@ -48801,7 +48801,7 @@
         <v>25</v>
       </c>
       <c r="J217" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K217">
         <v>10</v>
@@ -48865,27 +48865,27 @@
         <v>3.6428571428571456E-2</v>
       </c>
       <c r="M218">
-        <f t="shared" ref="M218" si="43">-SLOPE(D218:D224,$J$2:$J$8)</f>
+        <f t="shared" ref="M218" si="44">-SLOPE(D218:D224,$J$2:$J$8)</f>
         <v>2.7000000000000021E-2</v>
       </c>
       <c r="N218">
-        <f t="shared" ref="N218" si="44">-SLOPE(E218:E224,$J$2:$J$8)</f>
+        <f t="shared" ref="N218" si="45">-SLOPE(E218:E224,$J$2:$J$8)</f>
         <v>3.3000000000000029E-2</v>
       </c>
       <c r="O218">
-        <f t="shared" ref="O218" si="45">-SLOPE(F218:F224,$J$2:$J$8)</f>
+        <f t="shared" ref="O218" si="46">-SLOPE(F218:F224,$J$2:$J$8)</f>
         <v>3.7285714285714311E-2</v>
       </c>
       <c r="P218">
-        <f t="shared" ref="P218" si="46">-SLOPE(G218:G224,$J$2:$J$8)</f>
+        <f t="shared" ref="P218" si="47">-SLOPE(G218:G224,$J$2:$J$8)</f>
         <v>3.9000000000000028E-2</v>
       </c>
       <c r="Q218">
-        <f t="shared" ref="Q218" si="47">-SLOPE(H218:H224,$J$2:$J$8)</f>
+        <f t="shared" ref="Q218" si="48">-SLOPE(H218:H224,$J$2:$J$8)</f>
         <v>4.2857142857142892E-2</v>
       </c>
       <c r="R218">
-        <f t="shared" ref="R218" si="48">-SLOPE(I218:I224,$J$2:$J$8)</f>
+        <f t="shared" ref="R218" si="49">-SLOPE(I218:I224,$J$2:$J$8)</f>
         <v>2.4857142857142731E-2</v>
       </c>
     </row>
@@ -49587,7 +49587,7 @@
     </row>
     <row r="244" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>27</v>
@@ -49675,27 +49675,27 @@
         <v>4.1571428571428606E-2</v>
       </c>
       <c r="M245">
-        <f t="shared" ref="M245" si="49">-SLOPE(D245:D251,$J$2:$J$8)</f>
+        <f t="shared" ref="M245" si="50">-SLOPE(D245:D251,$J$2:$J$8)</f>
         <v>4.2857142857142885E-2</v>
       </c>
       <c r="N245">
-        <f t="shared" ref="N245" si="50">-SLOPE(E245:E251,$J$2:$J$8)</f>
+        <f t="shared" ref="N245" si="51">-SLOPE(E245:E251,$J$2:$J$8)</f>
         <v>4.1142857142857175E-2</v>
       </c>
       <c r="O245">
-        <f t="shared" ref="O245" si="51">-SLOPE(F245:F251,$J$2:$J$8)</f>
+        <f t="shared" ref="O245" si="52">-SLOPE(F245:F251,$J$2:$J$8)</f>
         <v>3.4285714285714308E-2</v>
       </c>
       <c r="P245">
-        <f t="shared" ref="P245" si="52">-SLOPE(G245:G251,$J$2:$J$8)</f>
+        <f t="shared" ref="P245" si="53">-SLOPE(G245:G251,$J$2:$J$8)</f>
         <v>5.1428571428571469E-2</v>
       </c>
       <c r="Q245">
-        <f t="shared" ref="Q245" si="53">-SLOPE(H245:H251,$J$2:$J$8)</f>
+        <f t="shared" ref="Q245" si="54">-SLOPE(H245:H251,$J$2:$J$8)</f>
         <v>3.7285714285714311E-2</v>
       </c>
       <c r="R245">
-        <f t="shared" ref="R245" si="54">-SLOPE(I245:I251,$J$2:$J$8)</f>
+        <f t="shared" ref="R245" si="55">-SLOPE(I245:I251,$J$2:$J$8)</f>
         <v>3.4285714285714308E-2</v>
       </c>
     </row>
@@ -50397,7 +50397,7 @@
     </row>
     <row r="271" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>36</v>
@@ -50485,27 +50485,27 @@
         <v>3.8571428571428604E-2</v>
       </c>
       <c r="M272">
-        <f t="shared" ref="M272" si="55">-SLOPE(D272:D278,$J$2:$J$8)</f>
+        <f t="shared" ref="M272" si="56">-SLOPE(D272:D278,$J$2:$J$8)</f>
         <v>2.2714285714285729E-2</v>
       </c>
       <c r="N272">
-        <f t="shared" ref="N272" si="56">-SLOPE(E272:E278,$J$2:$J$8)</f>
+        <f t="shared" ref="N272" si="57">-SLOPE(E272:E278,$J$2:$J$8)</f>
         <v>3.4285714285714319E-3</v>
       </c>
       <c r="O272">
-        <f t="shared" ref="O272" si="57">-SLOPE(F272:F278,$J$2:$J$8)</f>
+        <f t="shared" ref="O272" si="58">-SLOPE(F272:F278,$J$2:$J$8)</f>
         <v>4.3714285714285747E-2</v>
       </c>
       <c r="P272">
-        <f t="shared" ref="P272" si="58">-SLOPE(G272:G278,$J$2:$J$8)</f>
+        <f t="shared" ref="P272" si="59">-SLOPE(G272:G278,$J$2:$J$8)</f>
         <v>2.4428571428571445E-2</v>
       </c>
       <c r="Q272">
-        <f t="shared" ref="Q272" si="59">-SLOPE(H272:H278,$J$2:$J$8)</f>
+        <f t="shared" ref="Q272" si="60">-SLOPE(H272:H278,$J$2:$J$8)</f>
         <v>1.9285714285714302E-2</v>
       </c>
       <c r="R272">
-        <f t="shared" ref="R272" si="60">-SLOPE(I272:I278,$J$2:$J$8)</f>
+        <f t="shared" ref="R272" si="61">-SLOPE(I272:I278,$J$2:$J$8)</f>
         <v>3.2142857142857167E-2</v>
       </c>
     </row>
@@ -51207,7 +51207,7 @@
     </row>
     <row r="298" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>45</v>
@@ -51295,27 +51295,27 @@
         <v>2.9142857142857168E-2</v>
       </c>
       <c r="M299">
-        <f t="shared" ref="M299" si="61">-SLOPE(D299:D305,$J$2:$J$8)</f>
+        <f t="shared" ref="M299" si="62">-SLOPE(D299:D305,$J$2:$J$8)</f>
         <v>2.0571428571428588E-2</v>
       </c>
       <c r="N299">
-        <f t="shared" ref="N299" si="62">-SLOPE(E299:E305,$J$2:$J$8)</f>
+        <f t="shared" ref="N299" si="63">-SLOPE(E299:E305,$J$2:$J$8)</f>
         <v>2.7857142857142875E-2</v>
       </c>
       <c r="O299">
-        <f t="shared" ref="O299" si="63">-SLOPE(F299:F305,$J$2:$J$8)</f>
+        <f t="shared" ref="O299" si="64">-SLOPE(F299:F305,$J$2:$J$8)</f>
         <v>3.1285714285714306E-2</v>
       </c>
       <c r="P299">
-        <f t="shared" ref="P299" si="64">-SLOPE(G299:G305,$J$2:$J$8)</f>
+        <f t="shared" ref="P299" si="65">-SLOPE(G299:G305,$J$2:$J$8)</f>
         <v>3.1714285714285737E-2</v>
       </c>
       <c r="Q299">
-        <f t="shared" ref="Q299" si="65">-SLOPE(H299:H305,$J$2:$J$8)</f>
+        <f t="shared" ref="Q299" si="66">-SLOPE(H299:H305,$J$2:$J$8)</f>
         <v>3.38571428571426E-2</v>
       </c>
       <c r="R299">
-        <f t="shared" ref="R299" si="66">-SLOPE(I299:I305,$J$2:$J$8)</f>
+        <f t="shared" ref="R299" si="67">-SLOPE(I299:I305,$J$2:$J$8)</f>
         <v>1.7571428571428585E-2</v>
       </c>
     </row>
@@ -52017,7 +52017,7 @@
     </row>
     <row r="325" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>0</v>
@@ -52105,27 +52105,27 @@
         <v>7.5428571428571192E-2</v>
       </c>
       <c r="M326">
-        <f t="shared" ref="M326" si="67">-SLOPE(D326:D332,$J$2:$J$8)</f>
+        <f t="shared" ref="M326" si="68">-SLOPE(D326:D332,$J$2:$J$8)</f>
         <v>9.3428571428571208E-2</v>
       </c>
       <c r="N326">
-        <f t="shared" ref="N326" si="68">-SLOPE(E326:E332,$J$2:$J$8)</f>
+        <f t="shared" ref="N326" si="69">-SLOPE(E326:E332,$J$2:$J$8)</f>
         <v>6.1714285714285756E-2</v>
       </c>
       <c r="O326">
-        <f t="shared" ref="O326" si="69">-SLOPE(F326:F332,$J$2:$J$8)</f>
+        <f t="shared" ref="O326" si="70">-SLOPE(F326:F332,$J$2:$J$8)</f>
         <v>6.4714285714285613E-2</v>
       </c>
       <c r="P326">
-        <f t="shared" ref="P326" si="70">-SLOPE(G326:G332,$J$2:$J$8)</f>
+        <f t="shared" ref="P326" si="71">-SLOPE(G326:G332,$J$2:$J$8)</f>
         <v>5.09999999999999E-2</v>
       </c>
       <c r="Q326">
-        <f t="shared" ref="Q326" si="71">-SLOPE(H326:H332,$J$2:$J$8)</f>
+        <f t="shared" ref="Q326" si="72">-SLOPE(H326:H332,$J$2:$J$8)</f>
         <v>5.357142857142861E-2</v>
       </c>
       <c r="R326">
-        <f t="shared" ref="R326" si="72">-SLOPE(I326:I332,$J$2:$J$8)</f>
+        <f t="shared" ref="R326" si="73">-SLOPE(I326:I332,$J$2:$J$8)</f>
         <v>3.2142857142857167E-2</v>
       </c>
     </row>
@@ -52827,7 +52827,7 @@
     </row>
     <row r="352" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>8</v>
@@ -52915,27 +52915,27 @@
         <v>7.0714285714285618E-2</v>
       </c>
       <c r="M353">
-        <f t="shared" ref="M353" si="73">-SLOPE(D353:D359,$J$2:$J$8)</f>
+        <f t="shared" ref="M353" si="74">-SLOPE(D353:D359,$J$2:$J$8)</f>
         <v>7.9285714285714348E-2</v>
       </c>
       <c r="N353">
-        <f t="shared" ref="N353" si="74">-SLOPE(E353:E359,$J$2:$J$8)</f>
+        <f t="shared" ref="N353" si="75">-SLOPE(E353:E359,$J$2:$J$8)</f>
         <v>5.7857142857142899E-2</v>
       </c>
       <c r="O353">
-        <f t="shared" ref="O353" si="75">-SLOPE(F353:F359,$J$2:$J$8)</f>
+        <f t="shared" ref="O353" si="76">-SLOPE(F353:F359,$J$2:$J$8)</f>
         <v>5.7428571428571475E-2</v>
       </c>
       <c r="P353">
-        <f t="shared" ref="P353" si="76">-SLOPE(G353:G359,$J$2:$J$8)</f>
+        <f t="shared" ref="P353" si="77">-SLOPE(G353:G359,$J$2:$J$8)</f>
         <v>5.9571428571428477E-2</v>
       </c>
       <c r="Q353">
-        <f t="shared" ref="Q353" si="77">-SLOPE(H353:H359,$J$2:$J$8)</f>
+        <f t="shared" ref="Q353" si="78">-SLOPE(H353:H359,$J$2:$J$8)</f>
         <v>6.5999999999999809E-2</v>
       </c>
       <c r="R353">
-        <f t="shared" ref="R353" si="78">-SLOPE(I353:I359,$J$2:$J$8)</f>
+        <f t="shared" ref="R353" si="79">-SLOPE(I353:I359,$J$2:$J$8)</f>
         <v>4.628571428571418E-2</v>
       </c>
     </row>
@@ -53637,7 +53637,7 @@
     </row>
     <row r="379" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B379" s="1" t="s">
         <v>18</v>
@@ -53725,27 +53725,27 @@
         <v>0.12942857142857128</v>
       </c>
       <c r="M380">
-        <f t="shared" ref="M380" si="79">-SLOPE(D380:D386,$J$2:$J$8)</f>
+        <f t="shared" ref="M380" si="80">-SLOPE(D380:D386,$J$2:$J$8)</f>
         <v>8.9142857142856927E-2</v>
       </c>
       <c r="N380">
-        <f t="shared" ref="N380" si="80">-SLOPE(E380:E386,$J$2:$J$8)</f>
+        <f t="shared" ref="N380" si="81">-SLOPE(E380:E386,$J$2:$J$8)</f>
         <v>9.7285714285714087E-2</v>
       </c>
       <c r="O380">
-        <f t="shared" ref="O380" si="81">-SLOPE(F380:F386,$J$2:$J$8)</f>
+        <f t="shared" ref="O380" si="82">-SLOPE(F380:F386,$J$2:$J$8)</f>
         <v>9.1285714285714123E-2</v>
       </c>
       <c r="P380">
-        <f t="shared" ref="P380" si="82">-SLOPE(G380:G386,$J$2:$J$8)</f>
+        <f t="shared" ref="P380" si="83">-SLOPE(G380:G386,$J$2:$J$8)</f>
         <v>6.7714285714285533E-2</v>
       </c>
       <c r="Q380">
-        <f t="shared" ref="Q380" si="83">-SLOPE(H380:H386,$J$2:$J$8)</f>
+        <f t="shared" ref="Q380" si="84">-SLOPE(H380:H386,$J$2:$J$8)</f>
         <v>7.1999999999999773E-2</v>
       </c>
       <c r="R380">
-        <f t="shared" ref="R380" si="84">-SLOPE(I380:I386,$J$2:$J$8)</f>
+        <f t="shared" ref="R380" si="85">-SLOPE(I380:I386,$J$2:$J$8)</f>
         <v>7.6285714285714068E-2</v>
       </c>
     </row>
@@ -54447,7 +54447,7 @@
     </row>
     <row r="406" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B406" s="1" t="s">
         <v>27</v>
@@ -54535,27 +54535,27 @@
         <v>0.11271428571428552</v>
       </c>
       <c r="M407">
-        <f t="shared" ref="M407" si="85">-SLOPE(D407:D413,$J$2:$J$8)</f>
+        <f t="shared" ref="M407" si="86">-SLOPE(D407:D413,$J$2:$J$8)</f>
         <v>0.11957142857142843</v>
       </c>
       <c r="N407">
-        <f t="shared" ref="N407" si="86">-SLOPE(E407:E413,$J$2:$J$8)</f>
+        <f t="shared" ref="N407" si="87">-SLOPE(E407:E413,$J$2:$J$8)</f>
         <v>0.10157142857142866</v>
       </c>
       <c r="O407">
-        <f t="shared" ref="O407" si="87">-SLOPE(F407:F413,$J$2:$J$8)</f>
+        <f t="shared" ref="O407" si="88">-SLOPE(F407:F413,$J$2:$J$8)</f>
         <v>0.11999999999999984</v>
       </c>
       <c r="P407">
-        <f t="shared" ref="P407" si="88">-SLOPE(G407:G413,$J$2:$J$8)</f>
+        <f t="shared" ref="P407" si="89">-SLOPE(G407:G413,$J$2:$J$8)</f>
         <v>7.7142857142856916E-2</v>
       </c>
       <c r="Q407">
-        <f t="shared" ref="Q407" si="89">-SLOPE(H407:H413,$J$2:$J$8)</f>
+        <f t="shared" ref="Q407" si="90">-SLOPE(H407:H413,$J$2:$J$8)</f>
         <v>7.842857142857125E-2</v>
       </c>
       <c r="R407">
-        <f t="shared" ref="R407" si="90">-SLOPE(I407:I413,$J$2:$J$8)</f>
+        <f t="shared" ref="R407" si="91">-SLOPE(I407:I413,$J$2:$J$8)</f>
         <v>7.3714285714285482E-2</v>
       </c>
     </row>

</xml_diff>